<commit_message>
Updated Cheat Sheet Again.
Updated Cheat Sheet document again.
</commit_message>
<xml_diff>
--- a/public/ftpData/SuperDraft-SCCheatSheet2018.xlsx
+++ b/public/ftpData/SuperDraft-SCCheatSheet2018.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16300"/>
   </bookViews>
   <sheets>
     <sheet name="SC2018" sheetId="8" r:id="rId1"/>
@@ -3495,7 +3495,7 @@
   <dimension ref="A1:L827"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35933,6 +35933,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A9:E814"/>
   <mergeCells count="1">
     <mergeCell ref="D3:E3"/>

</xml_diff>